<commit_message>
Se actualiza el archivo
</commit_message>
<xml_diff>
--- a/MediK-V2/Control de peso.xlsx
+++ b/MediK-V2/Control de peso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XMY2729\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XMY2729\Documents\Pruebas_Concepto\Git\MediKProyect\MediK-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -226,10 +226,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$19</c:f>
+              <c:f>Hoja1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -283,16 +283,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>43707</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$19</c:f>
+              <c:f>Hoja1!$B$2:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>78.099999999999994</c:v>
                 </c:pt>
@@ -346,6 +349,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>68.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>69.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -658,10 +664,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$19</c:f>
+              <c:f>Hoja1!$A$2:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>43556</c:v>
                 </c:pt>
@@ -715,16 +721,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>43707</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$19</c:f>
+              <c:f>Hoja1!$C$2:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -775,6 +784,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>-0.54999999999999716</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3999999999999915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2364,10 +2376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2415,7 +2427,7 @@
         <v>76.45</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C19" si="0">-1*(B3-B4)</f>
+        <f t="shared" ref="C4:C20" si="0">-1*(B3-B4)</f>
         <v>-1.6499999999999915</v>
       </c>
     </row>
@@ -2597,6 +2609,18 @@
       <c r="C19">
         <f t="shared" si="0"/>
         <v>-0.54999999999999716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43721</v>
+      </c>
+      <c r="B20">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1.3999999999999915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>